<commit_message>
QA Env Urls Added to Excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/Excel_Lib/picapagesforscript.xlsx
+++ b/src/main/java/Excel_Lib/picapagesforscript.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin Lambert\Documents\Works\QE_Image\PicayWebsiteAutomation\src\main\java\Excel_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB863205-E3B1-44DF-A608-60B306377369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DDF65-98C2-4546-BEFA-63E2D0A8E857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{26C88561-E088-41D2-A2F5-2DD53971D7D8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{26C88561-E088-41D2-A2F5-2DD53971D7D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ProdURLS" sheetId="1" r:id="rId1"/>
+    <sheet name="QAEnv" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="285">
   <si>
     <t>URLs</t>
   </si>
@@ -465,6 +466,432 @@
   </si>
   <si>
     <t>https://picaysalpica.sysco.com/es/Products/Pork-Cracklins.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Tips-and-Trends.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Products.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Tips-and-Trends.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Products.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Tips-and-Trends/Sobremesa.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Acai-Ice-Cream-con-Queso-Cotija~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Achiote-Salmon-with-Chayote-Squash~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Ancho-Chocolate-Pots-de-Crema~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Arepas-Reina-Pepiada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Breaded-Beef-Tongue-Filled-with-Cheese~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Calamari-Basil-and-Prosciutto-Bruschetta~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Chicha-Morada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Ahi-Tuna-Poke-with-Mango-Ponzu-and-Tostones-~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Camarones-Borrachos~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Caribbean-Shrimp-Cocktail~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Ceviche-de-Pulpo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Chicharronada-Arepas~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Chifrijo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Chorizo-Monterey-Jack-Stuffed-Yuca-Cups~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Coconut-Horchata~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Ajiaco~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Cuban-Sandwich-Spring-Rolls~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Fried-Yuca-Cups-stuffed-with-Crab-Mango-Salad~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Gluten-Free-Bu%C3%B1uelos-with-Guava-Syrup~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Honey-Braised-Pork-Cheek-Empanadas-with-Chimichurri~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Huevos-Rancheros-with-Guacamole-in-Tortilla-Cups-~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Mole-Rojo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Peruvian-Steak-Anticuchos~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Plantain-Tres-Leches-Bread-Pudding~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Empanadas-Pabellon~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Grilled-Chicken-thigh-glazed-tequila-chile-ancho-sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Jicama-Gazpacho~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Plantain-Wrapped-Crab-Cakes~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Squash-Blossom-Chile-Relleno~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Sweet-Corn-Tamales-Fig-Syrup~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Guajillo-Sweet-Tea-with-Tequila~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Mole-Cake-with-Cherry-Ice-Cream-Tamarind-Sauce-and-Orange-Caramel~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Mussels-in-Malagueta-Pepper-Broth~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Panela-Cheese-in-Honey-Habanero-Sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Pasilla-Steak-Dry-Rub~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Plantain-Rolls-with-Strings-of-Caramelized-Aji-Cachucha~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Rocoto-Shrimp~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Street-Corn~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Tempura-Oysters-with-Aji-Amarillo-Sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Tiradito~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Bacon-infused-Michelada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Baked-Plantain-Boat~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Beef-Oxtail-Braised-with-Chorizo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Cheese-and-Passionfruit-Tequenos~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Cheesecake-with-Crema-Mexicana-and-Grilled-Fig~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Cuban-Mojo-Marinated-Suckling-Pork~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Grilled-Shrimp-with-Yuca-Escabeche~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Mondongo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Plantain-Sandwich-with-Beef-Cheek-Meat~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Russian-Beet-and-Potato-Salad-Wraps~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Shrimp-and-Pork-Cracklin-Ceviche~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Tamarind-Popsicles~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Banh-Mi-Huarache~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Cachapa~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Chicharron-de-Queso-with-Loroco-Guacamole~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Churro-Donut-with-Cajeta-Ice-Cream~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Duck-Ropa-Vieja~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Fish-and-Octopus-Choripan~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Flor-de-Calabaza-Stuffed-with-Goat-Cheese~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Juice-Flight~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Pan-de-Jamon~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Portobello-Lomo-Saltado~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Tres-Leches-Earl-Grey-Flan~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Recipes/Recipe~Creamy-poblano-pasta~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Products/Mexican-Cream.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/Products/Pork-Cracklins.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Tips-and-Trends/Sobremesa.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Acai-Ice-Cream-con-Queso-Cotija~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Achiote-Salmon-with-Chayote-Squash~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Ancho-Chocolate-Pots-de-Crema~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Arepas-Reina-Pepiada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Breaded-Beef-Tongue-Filled-with-Cheese~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Calamari-Basil-and-Prosciutto-Bruschetta~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Chicha-Morada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Ahi-Tuna-Poke-with-Mango-Ponzu-and-Tostones-~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Camarones-Borrachos~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Caribbean-Shrimp-Cocktail~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Ceviche-de-Pulpo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Chicharronada-Arepas~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Chifrijo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Chorizo-Monterey-Jack-Stuffed-Yuca-Cups~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Coconut-Horchata~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Ajiaco~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Cuban-Sandwich-Spring-Rolls~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Fried-Yuca-Cups-stuffed-with-Crab-Mango-Salad~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Gluten-Free-Bu%C3%B1uelos-with-Guava-Syrup~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Honey-Braised-Pork-Cheek-Empanadas-with-Chimichurri~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Huevos-Rancheros-with-Guacamole-in-Tortilla-Cups-~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Mole-Rojo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Peruvian-Steak-Anticuchos~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Plantain-Tres-Leches-Bread-Pudding~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Empanadas-Pabellon~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Grilled-Chicken-thigh-glazed-tequila-chile-ancho-sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Jicama-Gazpacho~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Plantain-Wrapped-Crab-Cakes~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Squash-Blossom-Chile-Relleno~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Sweet-Corn-Tamales-Fig-Syrup~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Guajillo-Sweet-Tea-with-Tequila~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Mole-Cake-with-Cherry-Ice-Cream-Tamarind-Sauce-and-Orange-Caramel~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Mussels-in-Malagueta-Pepper-Broth~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Panela-Cheese-in-Honey-Habanero-Sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Pasilla-Steak-Dry-Rub~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Plantain-Rolls-with-Strings-of-Caramelized-Aji-Cachucha~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Rocoto-Shrimp~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Street-Corn~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Tempura-Oysters-with-Aji-Amarillo-Sauce~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Tiradito~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Bacon-infused-Michelada~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Baked-Plantain-Boat~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Beef-Oxtail-Braised-with-Chorizo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Cheese-and-Passionfruit-Tequenos~.htm</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Cheesecake-with-Crema-Mexicana-and-Grilled-Fig~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Cuban-Mojo-Marinated-Suckling-Pork~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Grilled-Shrimp-with-Yuca-Escabeche~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Mondongo~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Plantain-Sandwich-with-Beef-Cheek-Meat~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Russian-Beet-and-Potato-Salad-Wraps~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Shrimp-and-Pork-Cracklin-Ceviche~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Tamarind-Popsicles~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Banh-Mi-Huarache~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Cachapa~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Chicharron-de-Queso-with-Loroco-Guacamole~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Churro-Donut-with-Cajeta-Ice-Cream~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Duck-Ropa-Vieja~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Fish-and-Octopus-Choripan~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Flor-de-Calabaza-Stuffed-with-Goat-Cheese~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Juice-Flight~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Pan-de-Jamon~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Portobello-Lomo-Saltado~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Tres-Leches-Earl-Grey-Flan~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Recipes/Recipe~Creamy-poblano-pasta~.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Products/Mexican-Cream.html</t>
+  </si>
+  <si>
+    <t>http://sysco-pica-y-salpica-qa.cxws-websites-nonprod.us-east-1.aws.sysco.net/es/Products/Pork-Cracklins.html</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1418,7 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1000,6 +1427,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1358,7 +1786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C84CCF-9446-4C8D-AAC4-A2AF5DABC089}">
   <dimension ref="A1:A144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2233,4 +2661,735 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId143"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF4242A-1035-4F34-BAE5-310CC44DDD22}">
+  <dimension ref="A1:A143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="131.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>